<commit_message>
First flow partially completed
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -4,60 +4,88 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13065" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18030" windowHeight="9930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
-    <sheet name="Smaple2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Functional" sheetId="2" r:id="rId2"/>
+    <sheet name="Zephyr 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:M18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
-  <si>
-    <t>Version name</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Test Case ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+  <si>
+    <t>testId</t>
+  </si>
+  <si>
+    <t>cyclename</t>
+  </si>
+  <si>
+    <t>version name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>TEMS-71</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Version 1.0</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TEMS-438</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Cycle Name</t>
+  </si>
+  <si>
+    <t>Version Name</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>TEMS-76</t>
   </si>
   <si>
-    <t>TEMS-71</t>
+    <t>TEMS-328</t>
+  </si>
+  <si>
+    <t>Functional</t>
   </si>
   <si>
     <t>Ver1.1</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cycle Name </t>
-  </si>
-  <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t>TEST-41</t>
-  </si>
-  <si>
-    <t>TEST-20</t>
-  </si>
-  <si>
-    <t>TEST-19</t>
-  </si>
-  <si>
-    <t>Version 1.0</t>
+    <t>TEMS-33</t>
+  </si>
+  <si>
+    <t>TEMS-32</t>
+  </si>
+  <si>
+    <t>TEMS-25</t>
+  </si>
+  <si>
+    <t>Zephyr 2</t>
+  </si>
+  <si>
+    <t>Vesrion 2.0</t>
   </si>
 </sst>
 </file>
@@ -73,41 +101,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -116,11 +123,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -424,128 +429,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -556,49 +566,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:D19"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>